<commit_message>
Example sheet for expenses
</commit_message>
<xml_diff>
--- a/backend/expense_details.xlsx
+++ b/backend/expense_details.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,18 +415,40 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Rent</v>
+        <v>celebrate</v>
       </c>
       <c r="B2">
-        <v>2500</v>
+        <v>23000</v>
       </c>
       <c r="C2" t="str">
+        <v>2025-05-01</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Cloths</v>
+      </c>
+      <c r="B3">
+        <v>3500</v>
+      </c>
+      <c r="C3" t="str">
         <v>2025-04-30</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Ice cream</v>
+      </c>
+      <c r="B4">
+        <v>130</v>
+      </c>
+      <c r="C4" t="str">
+        <v>2025-04-28</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added the resorse excel sheet
</commit_message>
<xml_diff>
--- a/backend/expense_details.xlsx
+++ b/backend/expense_details.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,40 +415,62 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>celebrate</v>
+        <v>popcorn</v>
       </c>
       <c r="B2">
-        <v>23000</v>
+        <v>500</v>
       </c>
       <c r="C2" t="str">
-        <v>2025-05-01</v>
+        <v>2025-05-04</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Cloths</v>
+        <v>Trouser</v>
       </c>
       <c r="B3">
-        <v>3500</v>
+        <v>4200</v>
       </c>
       <c r="C3" t="str">
-        <v>2025-04-30</v>
+        <v>2025-05-03</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Ice cream</v>
+        <v>Books</v>
       </c>
       <c r="B4">
-        <v>130</v>
+        <v>2850</v>
       </c>
       <c r="C4" t="str">
-        <v>2025-04-28</v>
+        <v>2025-05-02</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Celebration</v>
+      </c>
+      <c r="B5">
+        <v>1600</v>
+      </c>
+      <c r="C5" t="str">
+        <v>2025-05-01</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Film</v>
+      </c>
+      <c r="B6">
+        <v>1200</v>
+      </c>
+      <c r="C6" t="str">
+        <v>2025-04-29</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>